<commit_message>
[5_TuningPrompting][ASUITE gemini cần 3 cái xác thực] - KO PHẢI CHỈ MỖI gemini-api-key -)) nên là cần xử lý khác --- Còn OPENAI và GROD xử lý chung 1 kiểu
</commit_message>
<xml_diff>
--- a/5_TuningPrompting/example/input_data.xlsx
+++ b/5_TuningPrompting/example/input_data.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://husteduvn-my.sharepoint.com/personal/cuong_dn210141_sis_hust_edu_vn/Documents/GIT/BasicTasks_Prompting/TuningPrompting/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_FB3CFCAAAF8CFEEE0AED140AF2BC070891CBC83D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9CCF75F9-DF30-4972-8CF3-628278126E27}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="TestingPromptOnDataset" sheetId="1" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="TestingPromptOnDataset"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -46,20 +40,21 @@
     <t>conversation_history</t>
   </si>
   <si>
-    <t>[{"role":"assistant","content":"Chúng ta sẽ bắt đầu với cụm 'Thức dậy'. Hãy cùng mình nói cụm 'Thức dậy' bằng tiếng anh nha"},{"role":"user","content":"À, 'Brush teeth' hả?"},{"role":"assistant","content":"Nghe thú vị thế. Nhưng trước tiên cùng nhắc lại cụm 'Thức dậy' trước nhen: 'Wake up'"},{"role":"user","content":"wake up"},{"role":"assistant","content":"Đúng rồi, giờ chúng ta qua cụm tiếp theo nhé. Đánh răng."}]</t>
-  </si>
-  <si>
     <t xml:space="preserve">Tôi là Cường </t>
   </si>
   <si>
     <t>AI Assistant</t>
   </si>
+  <si>
+    <t>[{"role":"assistant","content":"Chúng ta sẽ bắt đầu với cụm 'Thức dậy'. Hãy cùng mình nói cụm 'Thức dậy' bằng tiếng anh nha"},{"role":"user","content":"À, 'Brush teeth' hả?"},{"role":"assistant","content":"Nghe thú vị thế. Nhưng trước tiên cùng nhắc lại cụm 'Thức dậy' trước nhen: 'Wake up'"},{"role":"user","content":"wake up"},{"role":"assistant","content":"Đúng rồi, giờ chúng ta qua cụm tiếp theo nhé. Đánh răng."}]</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -78,6 +73,12 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
@@ -102,17 +103,17 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFB7B7B7"/>
+        <fgColor rgb="FFb7b7b7"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFEA9999"/>
+        <fgColor rgb="FFea9999"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF93C47D"/>
+        <fgColor rgb="FF93c47d"/>
       </patternFill>
     </fill>
   </fills>
@@ -126,37 +127,37 @@
     </border>
     <border>
       <left style="medium">
-        <color rgb="FFCCCCCC"/>
+        <color rgb="FFcccccc"/>
       </left>
       <right style="medium">
-        <color rgb="FFCCCCCC"/>
+        <color rgb="FFcccccc"/>
       </right>
       <top style="medium">
-        <color rgb="FFCCCCCC"/>
+        <color rgb="FFcccccc"/>
       </top>
       <bottom style="medium">
-        <color rgb="FFCCCCCC"/>
+        <color rgb="FFcccccc"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color rgb="FFCCCCCC"/>
+        <color rgb="FFcccccc"/>
       </left>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
       <top style="medium">
-        <color rgb="FFCCCCCC"/>
+        <color rgb="FFcccccc"/>
       </top>
       <bottom style="medium">
-        <color rgb="FFCCCCCC"/>
+        <color rgb="FFcccccc"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color rgb="FFCCCCCC"/>
+        <color rgb="FFcccccc"/>
       </left>
       <right style="medium">
         <color rgb="FF000000"/>
@@ -181,52 +182,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -237,10 +235,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -278,71 +276,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -370,7 +368,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -393,11 +391,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -406,13 +404,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -422,7 +420,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -431,7 +429,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -440,7 +438,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -448,10 +446,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -516,27 +514,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:H286"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="13.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="43.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="11" width="34.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="10" width="43.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="11" width="29.719285714285714" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="40.5" customFormat="1" s="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -562,23 +560,23 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="1" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="164.25" customFormat="1" s="1">
       <c r="A2" s="7"/>
       <c r="B2" s="7"/>
       <c r="C2" s="8"/>
       <c r="D2" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
       <c r="G2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="20.25" customFormat="1" s="1">
       <c r="A3" s="7"/>
       <c r="B3" s="7"/>
       <c r="C3" s="8"/>
@@ -588,7 +586,7 @@
       <c r="G3" s="7"/>
       <c r="H3" s="8"/>
     </row>
-    <row r="4" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="20.25" customFormat="1" s="1">
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="8"/>
@@ -598,7 +596,7 @@
       <c r="G4" s="7"/>
       <c r="H4" s="8"/>
     </row>
-    <row r="5" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="20.25" customFormat="1" s="1">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="8"/>
@@ -608,7 +606,7 @@
       <c r="G5" s="7"/>
       <c r="H5" s="8"/>
     </row>
-    <row r="6" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="20.25" customFormat="1" s="1">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="8"/>
@@ -618,7 +616,7 @@
       <c r="G6" s="7"/>
       <c r="H6" s="8"/>
     </row>
-    <row r="7" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="20.25" customFormat="1" s="1">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="8"/>
@@ -628,7 +626,7 @@
       <c r="G7" s="7"/>
       <c r="H7" s="8"/>
     </row>
-    <row r="8" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="8"/>
@@ -638,7 +636,7 @@
       <c r="G8" s="7"/>
       <c r="H8" s="8"/>
     </row>
-    <row r="9" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="8"/>
@@ -648,7 +646,7 @@
       <c r="G9" s="7"/>
       <c r="H9" s="8"/>
     </row>
-    <row r="10" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="8"/>
@@ -658,7 +656,7 @@
       <c r="G10" s="7"/>
       <c r="H10" s="8"/>
     </row>
-    <row r="11" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="8"/>
@@ -668,7 +666,7 @@
       <c r="G11" s="7"/>
       <c r="H11" s="8"/>
     </row>
-    <row r="12" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="8"/>
@@ -678,7 +676,7 @@
       <c r="G12" s="7"/>
       <c r="H12" s="8"/>
     </row>
-    <row r="13" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="8"/>
@@ -688,7 +686,7 @@
       <c r="G13" s="7"/>
       <c r="H13" s="8"/>
     </row>
-    <row r="14" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="8"/>
@@ -698,7 +696,7 @@
       <c r="G14" s="7"/>
       <c r="H14" s="8"/>
     </row>
-    <row r="15" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="8"/>
@@ -708,7 +706,7 @@
       <c r="G15" s="7"/>
       <c r="H15" s="8"/>
     </row>
-    <row r="16" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="8"/>
@@ -718,7 +716,7 @@
       <c r="G16" s="7"/>
       <c r="H16" s="8"/>
     </row>
-    <row r="17" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="8"/>
@@ -728,7 +726,7 @@
       <c r="G17" s="7"/>
       <c r="H17" s="8"/>
     </row>
-    <row r="18" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="8"/>
@@ -738,7 +736,7 @@
       <c r="G18" s="7"/>
       <c r="H18" s="8"/>
     </row>
-    <row r="19" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="8"/>
@@ -748,7 +746,7 @@
       <c r="G19" s="7"/>
       <c r="H19" s="8"/>
     </row>
-    <row r="20" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="C20" s="8"/>
@@ -758,7 +756,7 @@
       <c r="G20" s="7"/>
       <c r="H20" s="8"/>
     </row>
-    <row r="21" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A21" s="7"/>
       <c r="B21" s="7"/>
       <c r="C21" s="8"/>
@@ -768,7 +766,7 @@
       <c r="G21" s="7"/>
       <c r="H21" s="8"/>
     </row>
-    <row r="22" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A22" s="7"/>
       <c r="B22" s="7"/>
       <c r="C22" s="8"/>
@@ -778,7 +776,7 @@
       <c r="G22" s="7"/>
       <c r="H22" s="8"/>
     </row>
-    <row r="23" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A23" s="7"/>
       <c r="B23" s="7"/>
       <c r="C23" s="8"/>
@@ -788,7 +786,7 @@
       <c r="G23" s="7"/>
       <c r="H23" s="8"/>
     </row>
-    <row r="24" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A24" s="7"/>
       <c r="B24" s="7"/>
       <c r="C24" s="8"/>
@@ -798,7 +796,7 @@
       <c r="G24" s="7"/>
       <c r="H24" s="8"/>
     </row>
-    <row r="25" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A25" s="7"/>
       <c r="B25" s="7"/>
       <c r="C25" s="8"/>
@@ -808,7 +806,7 @@
       <c r="G25" s="7"/>
       <c r="H25" s="8"/>
     </row>
-    <row r="26" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A26" s="7"/>
       <c r="B26" s="7"/>
       <c r="C26" s="8"/>
@@ -818,7 +816,7 @@
       <c r="G26" s="7"/>
       <c r="H26" s="8"/>
     </row>
-    <row r="27" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A27" s="7"/>
       <c r="B27" s="7"/>
       <c r="C27" s="8"/>
@@ -828,7 +826,7 @@
       <c r="G27" s="7"/>
       <c r="H27" s="8"/>
     </row>
-    <row r="28" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A28" s="7"/>
       <c r="B28" s="7"/>
       <c r="C28" s="8"/>
@@ -838,7 +836,7 @@
       <c r="G28" s="7"/>
       <c r="H28" s="8"/>
     </row>
-    <row r="29" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A29" s="7"/>
       <c r="B29" s="7"/>
       <c r="C29" s="8"/>
@@ -848,7 +846,7 @@
       <c r="G29" s="7"/>
       <c r="H29" s="8"/>
     </row>
-    <row r="30" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A30" s="7"/>
       <c r="B30" s="7"/>
       <c r="C30" s="8"/>
@@ -858,7 +856,7 @@
       <c r="G30" s="7"/>
       <c r="H30" s="8"/>
     </row>
-    <row r="31" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A31" s="7"/>
       <c r="B31" s="7"/>
       <c r="C31" s="8"/>
@@ -868,7 +866,7 @@
       <c r="G31" s="7"/>
       <c r="H31" s="8"/>
     </row>
-    <row r="32" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A32" s="7"/>
       <c r="B32" s="7"/>
       <c r="C32" s="8"/>
@@ -878,7 +876,7 @@
       <c r="G32" s="7"/>
       <c r="H32" s="8"/>
     </row>
-    <row r="33" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A33" s="7"/>
       <c r="B33" s="7"/>
       <c r="C33" s="8"/>
@@ -888,7 +886,7 @@
       <c r="G33" s="7"/>
       <c r="H33" s="8"/>
     </row>
-    <row r="34" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A34" s="7"/>
       <c r="B34" s="7"/>
       <c r="C34" s="8"/>
@@ -898,7 +896,7 @@
       <c r="G34" s="7"/>
       <c r="H34" s="8"/>
     </row>
-    <row r="35" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A35" s="7"/>
       <c r="B35" s="7"/>
       <c r="C35" s="8"/>
@@ -908,7 +906,7 @@
       <c r="G35" s="7"/>
       <c r="H35" s="8"/>
     </row>
-    <row r="36" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A36" s="7"/>
       <c r="B36" s="7"/>
       <c r="C36" s="8"/>
@@ -918,7 +916,7 @@
       <c r="G36" s="7"/>
       <c r="H36" s="8"/>
     </row>
-    <row r="37" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A37" s="7"/>
       <c r="B37" s="7"/>
       <c r="C37" s="8"/>
@@ -928,7 +926,7 @@
       <c r="G37" s="7"/>
       <c r="H37" s="8"/>
     </row>
-    <row r="38" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A38" s="7"/>
       <c r="B38" s="7"/>
       <c r="C38" s="8"/>
@@ -938,7 +936,7 @@
       <c r="G38" s="7"/>
       <c r="H38" s="8"/>
     </row>
-    <row r="39" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A39" s="7"/>
       <c r="B39" s="7"/>
       <c r="C39" s="8"/>
@@ -948,7 +946,7 @@
       <c r="G39" s="7"/>
       <c r="H39" s="8"/>
     </row>
-    <row r="40" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A40" s="7"/>
       <c r="B40" s="7"/>
       <c r="C40" s="8"/>
@@ -958,7 +956,7 @@
       <c r="G40" s="7"/>
       <c r="H40" s="8"/>
     </row>
-    <row r="41" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A41" s="7"/>
       <c r="B41" s="7"/>
       <c r="C41" s="8"/>
@@ -968,7 +966,7 @@
       <c r="G41" s="7"/>
       <c r="H41" s="8"/>
     </row>
-    <row r="42" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A42" s="7"/>
       <c r="B42" s="7"/>
       <c r="C42" s="8"/>
@@ -978,7 +976,7 @@
       <c r="G42" s="7"/>
       <c r="H42" s="8"/>
     </row>
-    <row r="43" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A43" s="7"/>
       <c r="B43" s="7"/>
       <c r="C43" s="8"/>
@@ -988,7 +986,7 @@
       <c r="G43" s="7"/>
       <c r="H43" s="8"/>
     </row>
-    <row r="44" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A44" s="7"/>
       <c r="B44" s="7"/>
       <c r="C44" s="8"/>
@@ -998,7 +996,7 @@
       <c r="G44" s="7"/>
       <c r="H44" s="8"/>
     </row>
-    <row r="45" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A45" s="7"/>
       <c r="B45" s="7"/>
       <c r="C45" s="8"/>
@@ -1008,7 +1006,7 @@
       <c r="G45" s="7"/>
       <c r="H45" s="8"/>
     </row>
-    <row r="46" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A46" s="7"/>
       <c r="B46" s="7"/>
       <c r="C46" s="8"/>
@@ -1018,7 +1016,7 @@
       <c r="G46" s="7"/>
       <c r="H46" s="8"/>
     </row>
-    <row r="47" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A47" s="7"/>
       <c r="B47" s="7"/>
       <c r="C47" s="8"/>
@@ -1028,7 +1026,7 @@
       <c r="G47" s="7"/>
       <c r="H47" s="8"/>
     </row>
-    <row r="48" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A48" s="7"/>
       <c r="B48" s="7"/>
       <c r="C48" s="8"/>
@@ -1038,7 +1036,7 @@
       <c r="G48" s="7"/>
       <c r="H48" s="8"/>
     </row>
-    <row r="49" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A49" s="7"/>
       <c r="B49" s="7"/>
       <c r="C49" s="8"/>
@@ -1048,7 +1046,7 @@
       <c r="G49" s="7"/>
       <c r="H49" s="8"/>
     </row>
-    <row r="50" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A50" s="7"/>
       <c r="B50" s="7"/>
       <c r="C50" s="8"/>
@@ -1058,7 +1056,7 @@
       <c r="G50" s="7"/>
       <c r="H50" s="8"/>
     </row>
-    <row r="51" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A51" s="7"/>
       <c r="B51" s="7"/>
       <c r="C51" s="8"/>
@@ -1068,7 +1066,7 @@
       <c r="G51" s="7"/>
       <c r="H51" s="8"/>
     </row>
-    <row r="52" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A52" s="7"/>
       <c r="B52" s="7"/>
       <c r="C52" s="8"/>
@@ -1078,7 +1076,7 @@
       <c r="G52" s="7"/>
       <c r="H52" s="8"/>
     </row>
-    <row r="53" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A53" s="7"/>
       <c r="B53" s="7"/>
       <c r="C53" s="8"/>
@@ -1088,7 +1086,7 @@
       <c r="G53" s="7"/>
       <c r="H53" s="8"/>
     </row>
-    <row r="54" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A54" s="7"/>
       <c r="B54" s="7"/>
       <c r="C54" s="8"/>
@@ -1098,7 +1096,7 @@
       <c r="G54" s="7"/>
       <c r="H54" s="8"/>
     </row>
-    <row r="55" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A55" s="7"/>
       <c r="B55" s="7"/>
       <c r="C55" s="8"/>
@@ -1108,7 +1106,7 @@
       <c r="G55" s="7"/>
       <c r="H55" s="8"/>
     </row>
-    <row r="56" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A56" s="7"/>
       <c r="B56" s="7"/>
       <c r="C56" s="8"/>
@@ -1118,7 +1116,7 @@
       <c r="G56" s="7"/>
       <c r="H56" s="8"/>
     </row>
-    <row r="57" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A57" s="7"/>
       <c r="B57" s="7"/>
       <c r="C57" s="8"/>
@@ -1128,7 +1126,7 @@
       <c r="G57" s="7"/>
       <c r="H57" s="8"/>
     </row>
-    <row r="58" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A58" s="7"/>
       <c r="B58" s="7"/>
       <c r="C58" s="8"/>
@@ -1138,7 +1136,7 @@
       <c r="G58" s="7"/>
       <c r="H58" s="8"/>
     </row>
-    <row r="59" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A59" s="7"/>
       <c r="B59" s="7"/>
       <c r="C59" s="8"/>
@@ -1148,7 +1146,7 @@
       <c r="G59" s="7"/>
       <c r="H59" s="8"/>
     </row>
-    <row r="60" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A60" s="7"/>
       <c r="B60" s="7"/>
       <c r="C60" s="8"/>
@@ -1158,7 +1156,7 @@
       <c r="G60" s="7"/>
       <c r="H60" s="8"/>
     </row>
-    <row r="61" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A61" s="7"/>
       <c r="B61" s="7"/>
       <c r="C61" s="8"/>
@@ -1168,7 +1166,7 @@
       <c r="G61" s="7"/>
       <c r="H61" s="8"/>
     </row>
-    <row r="62" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A62" s="7"/>
       <c r="B62" s="7"/>
       <c r="C62" s="8"/>
@@ -1178,7 +1176,7 @@
       <c r="G62" s="7"/>
       <c r="H62" s="8"/>
     </row>
-    <row r="63" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A63" s="7"/>
       <c r="B63" s="7"/>
       <c r="C63" s="8"/>
@@ -1188,7 +1186,7 @@
       <c r="G63" s="7"/>
       <c r="H63" s="8"/>
     </row>
-    <row r="64" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A64" s="7"/>
       <c r="B64" s="7"/>
       <c r="C64" s="8"/>
@@ -1198,7 +1196,7 @@
       <c r="G64" s="7"/>
       <c r="H64" s="8"/>
     </row>
-    <row r="65" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A65" s="7"/>
       <c r="B65" s="7"/>
       <c r="C65" s="8"/>
@@ -1208,7 +1206,7 @@
       <c r="G65" s="7"/>
       <c r="H65" s="8"/>
     </row>
-    <row r="66" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A66" s="7"/>
       <c r="B66" s="7"/>
       <c r="C66" s="8"/>
@@ -1218,7 +1216,7 @@
       <c r="G66" s="7"/>
       <c r="H66" s="8"/>
     </row>
-    <row r="67" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A67" s="7"/>
       <c r="B67" s="7"/>
       <c r="C67" s="8"/>
@@ -1228,7 +1226,7 @@
       <c r="G67" s="7"/>
       <c r="H67" s="8"/>
     </row>
-    <row r="68" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A68" s="7"/>
       <c r="B68" s="7"/>
       <c r="C68" s="8"/>
@@ -1238,7 +1236,7 @@
       <c r="G68" s="7"/>
       <c r="H68" s="8"/>
     </row>
-    <row r="69" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A69" s="7"/>
       <c r="B69" s="7"/>
       <c r="C69" s="8"/>
@@ -1248,7 +1246,7 @@
       <c r="G69" s="7"/>
       <c r="H69" s="8"/>
     </row>
-    <row r="70" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A70" s="7"/>
       <c r="B70" s="7"/>
       <c r="C70" s="8"/>
@@ -1258,7 +1256,7 @@
       <c r="G70" s="7"/>
       <c r="H70" s="8"/>
     </row>
-    <row r="71" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A71" s="7"/>
       <c r="B71" s="7"/>
       <c r="C71" s="8"/>
@@ -1268,7 +1266,7 @@
       <c r="G71" s="7"/>
       <c r="H71" s="8"/>
     </row>
-    <row r="72" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A72" s="7"/>
       <c r="B72" s="7"/>
       <c r="C72" s="8"/>
@@ -1278,7 +1276,7 @@
       <c r="G72" s="7"/>
       <c r="H72" s="8"/>
     </row>
-    <row r="73" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A73" s="7"/>
       <c r="B73" s="7"/>
       <c r="C73" s="8"/>
@@ -1288,7 +1286,7 @@
       <c r="G73" s="7"/>
       <c r="H73" s="8"/>
     </row>
-    <row r="74" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A74" s="7"/>
       <c r="B74" s="7"/>
       <c r="C74" s="8"/>
@@ -1298,7 +1296,7 @@
       <c r="G74" s="7"/>
       <c r="H74" s="8"/>
     </row>
-    <row r="75" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A75" s="7"/>
       <c r="B75" s="7"/>
       <c r="C75" s="8"/>
@@ -1308,7 +1306,7 @@
       <c r="G75" s="7"/>
       <c r="H75" s="8"/>
     </row>
-    <row r="76" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A76" s="7"/>
       <c r="B76" s="7"/>
       <c r="C76" s="8"/>
@@ -1318,7 +1316,7 @@
       <c r="G76" s="7"/>
       <c r="H76" s="8"/>
     </row>
-    <row r="77" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A77" s="7"/>
       <c r="B77" s="7"/>
       <c r="C77" s="8"/>
@@ -1328,7 +1326,7 @@
       <c r="G77" s="7"/>
       <c r="H77" s="8"/>
     </row>
-    <row r="78" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A78" s="7"/>
       <c r="B78" s="7"/>
       <c r="C78" s="8"/>
@@ -1338,7 +1336,7 @@
       <c r="G78" s="7"/>
       <c r="H78" s="8"/>
     </row>
-    <row r="79" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A79" s="7"/>
       <c r="B79" s="7"/>
       <c r="C79" s="8"/>
@@ -1348,7 +1346,7 @@
       <c r="G79" s="7"/>
       <c r="H79" s="8"/>
     </row>
-    <row r="80" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A80" s="7"/>
       <c r="B80" s="7"/>
       <c r="C80" s="8"/>
@@ -1358,7 +1356,7 @@
       <c r="G80" s="7"/>
       <c r="H80" s="8"/>
     </row>
-    <row r="81" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A81" s="7"/>
       <c r="B81" s="7"/>
       <c r="C81" s="8"/>
@@ -1368,7 +1366,7 @@
       <c r="G81" s="7"/>
       <c r="H81" s="8"/>
     </row>
-    <row r="82" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A82" s="7"/>
       <c r="B82" s="7"/>
       <c r="C82" s="8"/>
@@ -1378,7 +1376,7 @@
       <c r="G82" s="7"/>
       <c r="H82" s="8"/>
     </row>
-    <row r="83" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A83" s="7"/>
       <c r="B83" s="7"/>
       <c r="C83" s="8"/>
@@ -1388,7 +1386,7 @@
       <c r="G83" s="7"/>
       <c r="H83" s="8"/>
     </row>
-    <row r="84" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A84" s="7"/>
       <c r="B84" s="7"/>
       <c r="C84" s="8"/>
@@ -1398,7 +1396,7 @@
       <c r="G84" s="7"/>
       <c r="H84" s="8"/>
     </row>
-    <row r="85" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A85" s="7"/>
       <c r="B85" s="7"/>
       <c r="C85" s="8"/>
@@ -1408,7 +1406,7 @@
       <c r="G85" s="7"/>
       <c r="H85" s="8"/>
     </row>
-    <row r="86" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A86" s="7"/>
       <c r="B86" s="7"/>
       <c r="C86" s="8"/>
@@ -1418,7 +1416,7 @@
       <c r="G86" s="7"/>
       <c r="H86" s="8"/>
     </row>
-    <row r="87" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A87" s="7"/>
       <c r="B87" s="7"/>
       <c r="C87" s="8"/>
@@ -1428,7 +1426,7 @@
       <c r="G87" s="7"/>
       <c r="H87" s="8"/>
     </row>
-    <row r="88" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A88" s="7"/>
       <c r="B88" s="7"/>
       <c r="C88" s="8"/>
@@ -1438,7 +1436,7 @@
       <c r="G88" s="7"/>
       <c r="H88" s="8"/>
     </row>
-    <row r="89" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A89" s="7"/>
       <c r="B89" s="7"/>
       <c r="C89" s="8"/>
@@ -1448,7 +1446,7 @@
       <c r="G89" s="7"/>
       <c r="H89" s="8"/>
     </row>
-    <row r="90" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A90" s="7"/>
       <c r="B90" s="7"/>
       <c r="C90" s="8"/>
@@ -1458,7 +1456,7 @@
       <c r="G90" s="7"/>
       <c r="H90" s="8"/>
     </row>
-    <row r="91" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A91" s="7"/>
       <c r="B91" s="7"/>
       <c r="C91" s="8"/>
@@ -1468,7 +1466,7 @@
       <c r="G91" s="7"/>
       <c r="H91" s="8"/>
     </row>
-    <row r="92" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A92" s="7"/>
       <c r="B92" s="7"/>
       <c r="C92" s="8"/>
@@ -1478,7 +1476,7 @@
       <c r="G92" s="7"/>
       <c r="H92" s="8"/>
     </row>
-    <row r="93" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A93" s="7"/>
       <c r="B93" s="7"/>
       <c r="C93" s="8"/>
@@ -1488,7 +1486,7 @@
       <c r="G93" s="7"/>
       <c r="H93" s="8"/>
     </row>
-    <row r="94" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A94" s="7"/>
       <c r="B94" s="7"/>
       <c r="C94" s="8"/>
@@ -1498,7 +1496,7 @@
       <c r="G94" s="7"/>
       <c r="H94" s="8"/>
     </row>
-    <row r="95" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A95" s="7"/>
       <c r="B95" s="7"/>
       <c r="C95" s="8"/>
@@ -1508,7 +1506,7 @@
       <c r="G95" s="7"/>
       <c r="H95" s="8"/>
     </row>
-    <row r="96" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A96" s="7"/>
       <c r="B96" s="7"/>
       <c r="C96" s="8"/>
@@ -1518,7 +1516,7 @@
       <c r="G96" s="7"/>
       <c r="H96" s="8"/>
     </row>
-    <row r="97" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A97" s="7"/>
       <c r="B97" s="7"/>
       <c r="C97" s="8"/>
@@ -1528,7 +1526,7 @@
       <c r="G97" s="7"/>
       <c r="H97" s="8"/>
     </row>
-    <row r="98" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A98" s="7"/>
       <c r="B98" s="7"/>
       <c r="C98" s="8"/>
@@ -1538,7 +1536,7 @@
       <c r="G98" s="7"/>
       <c r="H98" s="8"/>
     </row>
-    <row r="99" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A99" s="7"/>
       <c r="B99" s="7"/>
       <c r="C99" s="8"/>
@@ -1548,7 +1546,7 @@
       <c r="G99" s="7"/>
       <c r="H99" s="8"/>
     </row>
-    <row r="100" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A100" s="7"/>
       <c r="B100" s="7"/>
       <c r="C100" s="8"/>
@@ -1558,7 +1556,7 @@
       <c r="G100" s="7"/>
       <c r="H100" s="8"/>
     </row>
-    <row r="101" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A101" s="7"/>
       <c r="B101" s="7"/>
       <c r="C101" s="8"/>
@@ -1568,7 +1566,7 @@
       <c r="G101" s="7"/>
       <c r="H101" s="8"/>
     </row>
-    <row r="102" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A102" s="7"/>
       <c r="B102" s="7"/>
       <c r="C102" s="8"/>
@@ -1578,7 +1576,7 @@
       <c r="G102" s="7"/>
       <c r="H102" s="8"/>
     </row>
-    <row r="103" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A103" s="7"/>
       <c r="B103" s="7"/>
       <c r="C103" s="8"/>
@@ -1588,7 +1586,7 @@
       <c r="G103" s="7"/>
       <c r="H103" s="8"/>
     </row>
-    <row r="104" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A104" s="7"/>
       <c r="B104" s="7"/>
       <c r="C104" s="8"/>
@@ -1598,7 +1596,7 @@
       <c r="G104" s="7"/>
       <c r="H104" s="8"/>
     </row>
-    <row r="105" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A105" s="7"/>
       <c r="B105" s="7"/>
       <c r="C105" s="8"/>
@@ -1608,7 +1606,7 @@
       <c r="G105" s="7"/>
       <c r="H105" s="8"/>
     </row>
-    <row r="106" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A106" s="7"/>
       <c r="B106" s="7"/>
       <c r="C106" s="8"/>
@@ -1618,7 +1616,7 @@
       <c r="G106" s="7"/>
       <c r="H106" s="8"/>
     </row>
-    <row r="107" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A107" s="7"/>
       <c r="B107" s="7"/>
       <c r="C107" s="8"/>
@@ -1628,7 +1626,7 @@
       <c r="G107" s="7"/>
       <c r="H107" s="8"/>
     </row>
-    <row r="108" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A108" s="7"/>
       <c r="B108" s="7"/>
       <c r="C108" s="8"/>
@@ -1638,7 +1636,7 @@
       <c r="G108" s="7"/>
       <c r="H108" s="8"/>
     </row>
-    <row r="109" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="109" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A109" s="7"/>
       <c r="B109" s="7"/>
       <c r="C109" s="8"/>
@@ -1648,7 +1646,7 @@
       <c r="G109" s="7"/>
       <c r="H109" s="8"/>
     </row>
-    <row r="110" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="110" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A110" s="7"/>
       <c r="B110" s="7"/>
       <c r="C110" s="8"/>
@@ -1658,7 +1656,7 @@
       <c r="G110" s="7"/>
       <c r="H110" s="8"/>
     </row>
-    <row r="111" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="111" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A111" s="7"/>
       <c r="B111" s="7"/>
       <c r="C111" s="8"/>
@@ -1668,7 +1666,7 @@
       <c r="G111" s="7"/>
       <c r="H111" s="8"/>
     </row>
-    <row r="112" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="112" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A112" s="7"/>
       <c r="B112" s="7"/>
       <c r="C112" s="8"/>
@@ -1678,7 +1676,7 @@
       <c r="G112" s="7"/>
       <c r="H112" s="8"/>
     </row>
-    <row r="113" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="113" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A113" s="7"/>
       <c r="B113" s="7"/>
       <c r="C113" s="8"/>
@@ -1688,7 +1686,7 @@
       <c r="G113" s="7"/>
       <c r="H113" s="8"/>
     </row>
-    <row r="114" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="114" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A114" s="7"/>
       <c r="B114" s="7"/>
       <c r="C114" s="8"/>
@@ -1698,7 +1696,7 @@
       <c r="G114" s="7"/>
       <c r="H114" s="8"/>
     </row>
-    <row r="115" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="115" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A115" s="7"/>
       <c r="B115" s="7"/>
       <c r="C115" s="8"/>
@@ -1708,7 +1706,7 @@
       <c r="G115" s="7"/>
       <c r="H115" s="8"/>
     </row>
-    <row r="116" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="116" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A116" s="7"/>
       <c r="B116" s="7"/>
       <c r="C116" s="8"/>
@@ -1718,7 +1716,7 @@
       <c r="G116" s="7"/>
       <c r="H116" s="8"/>
     </row>
-    <row r="117" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="117" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A117" s="7"/>
       <c r="B117" s="7"/>
       <c r="C117" s="8"/>
@@ -1728,7 +1726,7 @@
       <c r="G117" s="7"/>
       <c r="H117" s="8"/>
     </row>
-    <row r="118" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="118" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A118" s="7"/>
       <c r="B118" s="7"/>
       <c r="C118" s="8"/>
@@ -1738,7 +1736,7 @@
       <c r="G118" s="7"/>
       <c r="H118" s="8"/>
     </row>
-    <row r="119" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="119" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A119" s="7"/>
       <c r="B119" s="7"/>
       <c r="C119" s="8"/>
@@ -1748,7 +1746,7 @@
       <c r="G119" s="7"/>
       <c r="H119" s="8"/>
     </row>
-    <row r="120" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="120" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A120" s="7"/>
       <c r="B120" s="7"/>
       <c r="C120" s="8"/>
@@ -1758,7 +1756,7 @@
       <c r="G120" s="7"/>
       <c r="H120" s="8"/>
     </row>
-    <row r="121" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="121" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A121" s="7"/>
       <c r="B121" s="7"/>
       <c r="C121" s="8"/>
@@ -1768,7 +1766,7 @@
       <c r="G121" s="7"/>
       <c r="H121" s="8"/>
     </row>
-    <row r="122" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="122" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A122" s="7"/>
       <c r="B122" s="7"/>
       <c r="C122" s="8"/>
@@ -1778,7 +1776,7 @@
       <c r="G122" s="7"/>
       <c r="H122" s="8"/>
     </row>
-    <row r="123" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="123" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A123" s="7"/>
       <c r="B123" s="7"/>
       <c r="C123" s="8"/>
@@ -1788,7 +1786,7 @@
       <c r="G123" s="7"/>
       <c r="H123" s="8"/>
     </row>
-    <row r="124" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="124" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A124" s="7"/>
       <c r="B124" s="7"/>
       <c r="C124" s="8"/>
@@ -1798,7 +1796,7 @@
       <c r="G124" s="7"/>
       <c r="H124" s="8"/>
     </row>
-    <row r="125" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="125" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A125" s="7"/>
       <c r="B125" s="7"/>
       <c r="C125" s="8"/>
@@ -1808,7 +1806,7 @@
       <c r="G125" s="7"/>
       <c r="H125" s="8"/>
     </row>
-    <row r="126" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="126" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A126" s="7"/>
       <c r="B126" s="7"/>
       <c r="C126" s="8"/>
@@ -1818,7 +1816,7 @@
       <c r="G126" s="7"/>
       <c r="H126" s="8"/>
     </row>
-    <row r="127" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="127" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A127" s="7"/>
       <c r="B127" s="7"/>
       <c r="C127" s="8"/>
@@ -1828,7 +1826,7 @@
       <c r="G127" s="7"/>
       <c r="H127" s="8"/>
     </row>
-    <row r="128" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="128" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A128" s="7"/>
       <c r="B128" s="7"/>
       <c r="C128" s="8"/>
@@ -1838,7 +1836,7 @@
       <c r="G128" s="7"/>
       <c r="H128" s="8"/>
     </row>
-    <row r="129" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="129" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A129" s="7"/>
       <c r="B129" s="7"/>
       <c r="C129" s="8"/>
@@ -1848,7 +1846,7 @@
       <c r="G129" s="7"/>
       <c r="H129" s="8"/>
     </row>
-    <row r="130" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="130" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A130" s="7"/>
       <c r="B130" s="7"/>
       <c r="C130" s="8"/>
@@ -1858,7 +1856,7 @@
       <c r="G130" s="7"/>
       <c r="H130" s="8"/>
     </row>
-    <row r="131" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="131" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A131" s="7"/>
       <c r="B131" s="7"/>
       <c r="C131" s="8"/>
@@ -1868,7 +1866,7 @@
       <c r="G131" s="7"/>
       <c r="H131" s="8"/>
     </row>
-    <row r="132" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="132" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A132" s="7"/>
       <c r="B132" s="7"/>
       <c r="C132" s="8"/>
@@ -1878,7 +1876,7 @@
       <c r="G132" s="7"/>
       <c r="H132" s="8"/>
     </row>
-    <row r="133" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="133" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A133" s="7"/>
       <c r="B133" s="7"/>
       <c r="C133" s="8"/>
@@ -1888,7 +1886,7 @@
       <c r="G133" s="7"/>
       <c r="H133" s="8"/>
     </row>
-    <row r="134" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="134" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A134" s="7"/>
       <c r="B134" s="7"/>
       <c r="C134" s="8"/>
@@ -1898,7 +1896,7 @@
       <c r="G134" s="7"/>
       <c r="H134" s="8"/>
     </row>
-    <row r="135" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="135" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A135" s="7"/>
       <c r="B135" s="7"/>
       <c r="C135" s="8"/>
@@ -1908,7 +1906,7 @@
       <c r="G135" s="7"/>
       <c r="H135" s="8"/>
     </row>
-    <row r="136" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="136" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A136" s="7"/>
       <c r="B136" s="7"/>
       <c r="C136" s="8"/>
@@ -1918,7 +1916,7 @@
       <c r="G136" s="7"/>
       <c r="H136" s="8"/>
     </row>
-    <row r="137" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="137" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A137" s="7"/>
       <c r="B137" s="7"/>
       <c r="C137" s="8"/>
@@ -1928,7 +1926,7 @@
       <c r="G137" s="7"/>
       <c r="H137" s="8"/>
     </row>
-    <row r="138" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="138" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A138" s="7"/>
       <c r="B138" s="7"/>
       <c r="C138" s="8"/>
@@ -1938,7 +1936,7 @@
       <c r="G138" s="7"/>
       <c r="H138" s="8"/>
     </row>
-    <row r="139" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="139" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A139" s="7"/>
       <c r="B139" s="7"/>
       <c r="C139" s="8"/>
@@ -1948,7 +1946,7 @@
       <c r="G139" s="7"/>
       <c r="H139" s="8"/>
     </row>
-    <row r="140" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="140" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A140" s="7"/>
       <c r="B140" s="7"/>
       <c r="C140" s="8"/>
@@ -1958,7 +1956,7 @@
       <c r="G140" s="7"/>
       <c r="H140" s="8"/>
     </row>
-    <row r="141" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="141" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A141" s="7"/>
       <c r="B141" s="7"/>
       <c r="C141" s="8"/>
@@ -1968,7 +1966,7 @@
       <c r="G141" s="7"/>
       <c r="H141" s="8"/>
     </row>
-    <row r="142" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="142" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A142" s="7"/>
       <c r="B142" s="7"/>
       <c r="C142" s="8"/>
@@ -1978,7 +1976,7 @@
       <c r="G142" s="7"/>
       <c r="H142" s="8"/>
     </row>
-    <row r="143" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="143" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A143" s="7"/>
       <c r="B143" s="7"/>
       <c r="C143" s="8"/>
@@ -1988,7 +1986,7 @@
       <c r="G143" s="7"/>
       <c r="H143" s="8"/>
     </row>
-    <row r="144" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="144" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A144" s="7"/>
       <c r="B144" s="7"/>
       <c r="C144" s="8"/>
@@ -1998,7 +1996,7 @@
       <c r="G144" s="7"/>
       <c r="H144" s="8"/>
     </row>
-    <row r="145" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="145" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A145" s="7"/>
       <c r="B145" s="7"/>
       <c r="C145" s="8"/>
@@ -2008,7 +2006,7 @@
       <c r="G145" s="7"/>
       <c r="H145" s="8"/>
     </row>
-    <row r="146" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="146" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A146" s="7"/>
       <c r="B146" s="7"/>
       <c r="C146" s="8"/>
@@ -2018,7 +2016,7 @@
       <c r="G146" s="7"/>
       <c r="H146" s="8"/>
     </row>
-    <row r="147" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="147" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A147" s="7"/>
       <c r="B147" s="7"/>
       <c r="C147" s="8"/>
@@ -2028,7 +2026,7 @@
       <c r="G147" s="7"/>
       <c r="H147" s="8"/>
     </row>
-    <row r="148" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="148" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A148" s="7"/>
       <c r="B148" s="7"/>
       <c r="C148" s="8"/>
@@ -2038,7 +2036,7 @@
       <c r="G148" s="7"/>
       <c r="H148" s="8"/>
     </row>
-    <row r="149" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="149" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A149" s="7"/>
       <c r="B149" s="7"/>
       <c r="C149" s="8"/>
@@ -2048,7 +2046,7 @@
       <c r="G149" s="7"/>
       <c r="H149" s="8"/>
     </row>
-    <row r="150" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="150" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A150" s="7"/>
       <c r="B150" s="7"/>
       <c r="C150" s="8"/>
@@ -2058,7 +2056,7 @@
       <c r="G150" s="7"/>
       <c r="H150" s="8"/>
     </row>
-    <row r="151" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="151" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A151" s="7"/>
       <c r="B151" s="7"/>
       <c r="C151" s="8"/>
@@ -2068,7 +2066,7 @@
       <c r="G151" s="7"/>
       <c r="H151" s="8"/>
     </row>
-    <row r="152" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="152" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A152" s="7"/>
       <c r="B152" s="7"/>
       <c r="C152" s="8"/>
@@ -2078,7 +2076,7 @@
       <c r="G152" s="7"/>
       <c r="H152" s="8"/>
     </row>
-    <row r="153" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="153" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A153" s="7"/>
       <c r="B153" s="7"/>
       <c r="C153" s="8"/>
@@ -2088,7 +2086,7 @@
       <c r="G153" s="7"/>
       <c r="H153" s="8"/>
     </row>
-    <row r="154" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="154" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A154" s="7"/>
       <c r="B154" s="7"/>
       <c r="C154" s="8"/>
@@ -2098,7 +2096,7 @@
       <c r="G154" s="7"/>
       <c r="H154" s="8"/>
     </row>
-    <row r="155" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="155" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A155" s="7"/>
       <c r="B155" s="7"/>
       <c r="C155" s="8"/>
@@ -2108,7 +2106,7 @@
       <c r="G155" s="7"/>
       <c r="H155" s="8"/>
     </row>
-    <row r="156" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="156" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A156" s="7"/>
       <c r="B156" s="7"/>
       <c r="C156" s="8"/>
@@ -2118,7 +2116,7 @@
       <c r="G156" s="7"/>
       <c r="H156" s="8"/>
     </row>
-    <row r="157" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="157" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A157" s="7"/>
       <c r="B157" s="7"/>
       <c r="C157" s="8"/>
@@ -2128,7 +2126,7 @@
       <c r="G157" s="7"/>
       <c r="H157" s="8"/>
     </row>
-    <row r="158" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="158" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A158" s="7"/>
       <c r="B158" s="7"/>
       <c r="C158" s="8"/>
@@ -2138,7 +2136,7 @@
       <c r="G158" s="7"/>
       <c r="H158" s="8"/>
     </row>
-    <row r="159" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="159" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A159" s="7"/>
       <c r="B159" s="7"/>
       <c r="C159" s="8"/>
@@ -2148,7 +2146,7 @@
       <c r="G159" s="7"/>
       <c r="H159" s="8"/>
     </row>
-    <row r="160" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="160" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A160" s="7"/>
       <c r="B160" s="7"/>
       <c r="C160" s="8"/>
@@ -2158,7 +2156,7 @@
       <c r="G160" s="7"/>
       <c r="H160" s="8"/>
     </row>
-    <row r="161" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="161" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A161" s="7"/>
       <c r="B161" s="7"/>
       <c r="C161" s="8"/>
@@ -2168,7 +2166,7 @@
       <c r="G161" s="7"/>
       <c r="H161" s="8"/>
     </row>
-    <row r="162" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="162" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A162" s="7"/>
       <c r="B162" s="7"/>
       <c r="C162" s="8"/>
@@ -2178,7 +2176,7 @@
       <c r="G162" s="7"/>
       <c r="H162" s="8"/>
     </row>
-    <row r="163" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="163" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A163" s="7"/>
       <c r="B163" s="7"/>
       <c r="C163" s="8"/>
@@ -2188,7 +2186,7 @@
       <c r="G163" s="7"/>
       <c r="H163" s="8"/>
     </row>
-    <row r="164" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="164" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A164" s="7"/>
       <c r="B164" s="7"/>
       <c r="C164" s="8"/>
@@ -2198,7 +2196,7 @@
       <c r="G164" s="7"/>
       <c r="H164" s="8"/>
     </row>
-    <row r="165" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="165" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A165" s="7"/>
       <c r="B165" s="7"/>
       <c r="C165" s="8"/>
@@ -2208,7 +2206,7 @@
       <c r="G165" s="7"/>
       <c r="H165" s="8"/>
     </row>
-    <row r="166" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="166" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A166" s="7"/>
       <c r="B166" s="7"/>
       <c r="C166" s="8"/>
@@ -2218,7 +2216,7 @@
       <c r="G166" s="7"/>
       <c r="H166" s="8"/>
     </row>
-    <row r="167" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="167" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A167" s="7"/>
       <c r="B167" s="7"/>
       <c r="C167" s="8"/>
@@ -2228,7 +2226,7 @@
       <c r="G167" s="7"/>
       <c r="H167" s="8"/>
     </row>
-    <row r="168" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="168" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A168" s="7"/>
       <c r="B168" s="7"/>
       <c r="C168" s="8"/>
@@ -2238,7 +2236,7 @@
       <c r="G168" s="7"/>
       <c r="H168" s="8"/>
     </row>
-    <row r="169" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="169" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A169" s="7"/>
       <c r="B169" s="7"/>
       <c r="C169" s="8"/>
@@ -2248,7 +2246,7 @@
       <c r="G169" s="7"/>
       <c r="H169" s="8"/>
     </row>
-    <row r="170" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="170" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A170" s="7"/>
       <c r="B170" s="7"/>
       <c r="C170" s="8"/>
@@ -2258,7 +2256,7 @@
       <c r="G170" s="7"/>
       <c r="H170" s="8"/>
     </row>
-    <row r="171" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="171" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A171" s="7"/>
       <c r="B171" s="7"/>
       <c r="C171" s="8"/>
@@ -2268,7 +2266,7 @@
       <c r="G171" s="7"/>
       <c r="H171" s="8"/>
     </row>
-    <row r="172" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="172" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A172" s="7"/>
       <c r="B172" s="7"/>
       <c r="C172" s="8"/>
@@ -2278,7 +2276,7 @@
       <c r="G172" s="7"/>
       <c r="H172" s="8"/>
     </row>
-    <row r="173" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="173" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A173" s="7"/>
       <c r="B173" s="7"/>
       <c r="C173" s="8"/>
@@ -2288,7 +2286,7 @@
       <c r="G173" s="7"/>
       <c r="H173" s="8"/>
     </row>
-    <row r="174" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="174" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A174" s="7"/>
       <c r="B174" s="7"/>
       <c r="C174" s="8"/>
@@ -2298,7 +2296,7 @@
       <c r="G174" s="7"/>
       <c r="H174" s="8"/>
     </row>
-    <row r="175" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="175" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A175" s="7"/>
       <c r="B175" s="7"/>
       <c r="C175" s="8"/>
@@ -2308,7 +2306,7 @@
       <c r="G175" s="7"/>
       <c r="H175" s="8"/>
     </row>
-    <row r="176" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="176" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A176" s="7"/>
       <c r="B176" s="7"/>
       <c r="C176" s="8"/>
@@ -2318,7 +2316,7 @@
       <c r="G176" s="7"/>
       <c r="H176" s="8"/>
     </row>
-    <row r="177" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="177" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A177" s="7"/>
       <c r="B177" s="7"/>
       <c r="C177" s="8"/>
@@ -2328,7 +2326,7 @@
       <c r="G177" s="7"/>
       <c r="H177" s="8"/>
     </row>
-    <row r="178" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="178" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A178" s="7"/>
       <c r="B178" s="7"/>
       <c r="C178" s="8"/>
@@ -2338,7 +2336,7 @@
       <c r="G178" s="7"/>
       <c r="H178" s="8"/>
     </row>
-    <row r="179" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="179" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A179" s="7"/>
       <c r="B179" s="7"/>
       <c r="C179" s="8"/>
@@ -2348,7 +2346,7 @@
       <c r="G179" s="7"/>
       <c r="H179" s="8"/>
     </row>
-    <row r="180" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="180" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A180" s="7"/>
       <c r="B180" s="7"/>
       <c r="C180" s="8"/>
@@ -2358,7 +2356,7 @@
       <c r="G180" s="7"/>
       <c r="H180" s="8"/>
     </row>
-    <row r="181" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="181" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A181" s="7"/>
       <c r="B181" s="7"/>
       <c r="C181" s="8"/>
@@ -2368,7 +2366,7 @@
       <c r="G181" s="7"/>
       <c r="H181" s="8"/>
     </row>
-    <row r="182" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="182" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A182" s="7"/>
       <c r="B182" s="7"/>
       <c r="C182" s="8"/>
@@ -2378,7 +2376,7 @@
       <c r="G182" s="7"/>
       <c r="H182" s="8"/>
     </row>
-    <row r="183" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="183" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A183" s="7"/>
       <c r="B183" s="7"/>
       <c r="C183" s="8"/>
@@ -2388,7 +2386,7 @@
       <c r="G183" s="7"/>
       <c r="H183" s="8"/>
     </row>
-    <row r="184" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="184" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A184" s="7"/>
       <c r="B184" s="7"/>
       <c r="C184" s="8"/>
@@ -2398,7 +2396,7 @@
       <c r="G184" s="7"/>
       <c r="H184" s="8"/>
     </row>
-    <row r="185" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="185" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A185" s="7"/>
       <c r="B185" s="7"/>
       <c r="C185" s="8"/>
@@ -2408,7 +2406,7 @@
       <c r="G185" s="7"/>
       <c r="H185" s="8"/>
     </row>
-    <row r="186" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="186" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A186" s="7"/>
       <c r="B186" s="7"/>
       <c r="C186" s="8"/>
@@ -2418,7 +2416,7 @@
       <c r="G186" s="7"/>
       <c r="H186" s="8"/>
     </row>
-    <row r="187" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="187" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A187" s="7"/>
       <c r="B187" s="7"/>
       <c r="C187" s="8"/>
@@ -2428,7 +2426,7 @@
       <c r="G187" s="7"/>
       <c r="H187" s="8"/>
     </row>
-    <row r="188" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="188" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A188" s="7"/>
       <c r="B188" s="7"/>
       <c r="C188" s="8"/>
@@ -2438,7 +2436,7 @@
       <c r="G188" s="7"/>
       <c r="H188" s="8"/>
     </row>
-    <row r="189" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="189" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A189" s="7"/>
       <c r="B189" s="7"/>
       <c r="C189" s="8"/>
@@ -2448,7 +2446,7 @@
       <c r="G189" s="7"/>
       <c r="H189" s="8"/>
     </row>
-    <row r="190" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="190" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A190" s="7"/>
       <c r="B190" s="7"/>
       <c r="C190" s="8"/>
@@ -2458,7 +2456,7 @@
       <c r="G190" s="7"/>
       <c r="H190" s="8"/>
     </row>
-    <row r="191" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="191" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A191" s="7"/>
       <c r="B191" s="7"/>
       <c r="C191" s="8"/>
@@ -2468,7 +2466,7 @@
       <c r="G191" s="7"/>
       <c r="H191" s="8"/>
     </row>
-    <row r="192" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="192" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A192" s="7"/>
       <c r="B192" s="7"/>
       <c r="C192" s="8"/>
@@ -2478,7 +2476,7 @@
       <c r="G192" s="7"/>
       <c r="H192" s="8"/>
     </row>
-    <row r="193" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="193" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A193" s="7"/>
       <c r="B193" s="7"/>
       <c r="C193" s="8"/>
@@ -2488,7 +2486,7 @@
       <c r="G193" s="7"/>
       <c r="H193" s="8"/>
     </row>
-    <row r="194" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="194" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A194" s="7"/>
       <c r="B194" s="7"/>
       <c r="C194" s="8"/>
@@ -2498,7 +2496,7 @@
       <c r="G194" s="7"/>
       <c r="H194" s="8"/>
     </row>
-    <row r="195" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="195" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A195" s="7"/>
       <c r="B195" s="7"/>
       <c r="C195" s="8"/>
@@ -2508,7 +2506,7 @@
       <c r="G195" s="7"/>
       <c r="H195" s="8"/>
     </row>
-    <row r="196" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="196" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A196" s="7"/>
       <c r="B196" s="7"/>
       <c r="C196" s="8"/>
@@ -2518,7 +2516,7 @@
       <c r="G196" s="7"/>
       <c r="H196" s="8"/>
     </row>
-    <row r="197" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="197" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A197" s="7"/>
       <c r="B197" s="7"/>
       <c r="C197" s="8"/>
@@ -2528,7 +2526,7 @@
       <c r="G197" s="7"/>
       <c r="H197" s="8"/>
     </row>
-    <row r="198" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="198" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A198" s="7"/>
       <c r="B198" s="7"/>
       <c r="C198" s="8"/>
@@ -2538,7 +2536,7 @@
       <c r="G198" s="7"/>
       <c r="H198" s="8"/>
     </row>
-    <row r="199" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="199" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A199" s="7"/>
       <c r="B199" s="7"/>
       <c r="C199" s="8"/>
@@ -2548,7 +2546,7 @@
       <c r="G199" s="7"/>
       <c r="H199" s="8"/>
     </row>
-    <row r="200" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="200" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A200" s="7"/>
       <c r="B200" s="7"/>
       <c r="C200" s="8"/>
@@ -2558,7 +2556,7 @@
       <c r="G200" s="7"/>
       <c r="H200" s="8"/>
     </row>
-    <row r="201" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="201" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A201" s="7"/>
       <c r="B201" s="7"/>
       <c r="C201" s="8"/>
@@ -2568,7 +2566,7 @@
       <c r="G201" s="7"/>
       <c r="H201" s="8"/>
     </row>
-    <row r="202" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="202" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A202" s="7"/>
       <c r="B202" s="7"/>
       <c r="C202" s="8"/>
@@ -2578,7 +2576,7 @@
       <c r="G202" s="7"/>
       <c r="H202" s="8"/>
     </row>
-    <row r="203" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="203" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A203" s="7"/>
       <c r="B203" s="7"/>
       <c r="C203" s="8"/>
@@ -2588,7 +2586,7 @@
       <c r="G203" s="7"/>
       <c r="H203" s="8"/>
     </row>
-    <row r="204" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="204" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A204" s="7"/>
       <c r="B204" s="7"/>
       <c r="C204" s="8"/>
@@ -2598,7 +2596,7 @@
       <c r="G204" s="7"/>
       <c r="H204" s="8"/>
     </row>
-    <row r="205" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="205" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A205" s="7"/>
       <c r="B205" s="7"/>
       <c r="C205" s="8"/>
@@ -2608,7 +2606,7 @@
       <c r="G205" s="7"/>
       <c r="H205" s="8"/>
     </row>
-    <row r="206" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="206" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A206" s="7"/>
       <c r="B206" s="7"/>
       <c r="C206" s="8"/>
@@ -2618,7 +2616,7 @@
       <c r="G206" s="7"/>
       <c r="H206" s="8"/>
     </row>
-    <row r="207" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="207" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A207" s="7"/>
       <c r="B207" s="7"/>
       <c r="C207" s="8"/>
@@ -2628,7 +2626,7 @@
       <c r="G207" s="7"/>
       <c r="H207" s="8"/>
     </row>
-    <row r="208" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="208" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A208" s="7"/>
       <c r="B208" s="7"/>
       <c r="C208" s="8"/>
@@ -2638,7 +2636,7 @@
       <c r="G208" s="7"/>
       <c r="H208" s="8"/>
     </row>
-    <row r="209" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="209" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A209" s="7"/>
       <c r="B209" s="7"/>
       <c r="C209" s="8"/>
@@ -2648,7 +2646,7 @@
       <c r="G209" s="7"/>
       <c r="H209" s="8"/>
     </row>
-    <row r="210" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="210" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A210" s="7"/>
       <c r="B210" s="7"/>
       <c r="C210" s="8"/>
@@ -2658,7 +2656,7 @@
       <c r="G210" s="7"/>
       <c r="H210" s="8"/>
     </row>
-    <row r="211" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="211" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A211" s="7"/>
       <c r="B211" s="7"/>
       <c r="C211" s="8"/>
@@ -2668,7 +2666,7 @@
       <c r="G211" s="7"/>
       <c r="H211" s="8"/>
     </row>
-    <row r="212" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="212" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A212" s="7"/>
       <c r="B212" s="7"/>
       <c r="C212" s="8"/>
@@ -2678,7 +2676,7 @@
       <c r="G212" s="7"/>
       <c r="H212" s="8"/>
     </row>
-    <row r="213" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="213" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A213" s="7"/>
       <c r="B213" s="7"/>
       <c r="C213" s="8"/>
@@ -2688,7 +2686,7 @@
       <c r="G213" s="7"/>
       <c r="H213" s="8"/>
     </row>
-    <row r="214" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="214" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A214" s="7"/>
       <c r="B214" s="7"/>
       <c r="C214" s="8"/>
@@ -2698,7 +2696,7 @@
       <c r="G214" s="7"/>
       <c r="H214" s="8"/>
     </row>
-    <row r="215" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="215" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A215" s="7"/>
       <c r="B215" s="7"/>
       <c r="C215" s="8"/>
@@ -2708,7 +2706,7 @@
       <c r="G215" s="7"/>
       <c r="H215" s="8"/>
     </row>
-    <row r="216" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="216" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A216" s="7"/>
       <c r="B216" s="7"/>
       <c r="C216" s="8"/>
@@ -2718,7 +2716,7 @@
       <c r="G216" s="7"/>
       <c r="H216" s="8"/>
     </row>
-    <row r="217" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="217" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A217" s="7"/>
       <c r="B217" s="7"/>
       <c r="C217" s="8"/>
@@ -2728,7 +2726,7 @@
       <c r="G217" s="7"/>
       <c r="H217" s="8"/>
     </row>
-    <row r="218" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="218" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A218" s="7"/>
       <c r="B218" s="7"/>
       <c r="C218" s="8"/>
@@ -2738,7 +2736,7 @@
       <c r="G218" s="7"/>
       <c r="H218" s="8"/>
     </row>
-    <row r="219" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="219" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A219" s="7"/>
       <c r="B219" s="7"/>
       <c r="C219" s="8"/>
@@ -2748,7 +2746,7 @@
       <c r="G219" s="7"/>
       <c r="H219" s="8"/>
     </row>
-    <row r="220" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="220" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A220" s="7"/>
       <c r="B220" s="7"/>
       <c r="C220" s="8"/>
@@ -2758,7 +2756,7 @@
       <c r="G220" s="7"/>
       <c r="H220" s="8"/>
     </row>
-    <row r="221" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="221" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A221" s="7"/>
       <c r="B221" s="7"/>
       <c r="C221" s="8"/>
@@ -2768,7 +2766,7 @@
       <c r="G221" s="7"/>
       <c r="H221" s="8"/>
     </row>
-    <row r="222" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="222" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A222" s="7"/>
       <c r="B222" s="7"/>
       <c r="C222" s="8"/>
@@ -2778,7 +2776,7 @@
       <c r="G222" s="7"/>
       <c r="H222" s="8"/>
     </row>
-    <row r="223" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="223" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A223" s="7"/>
       <c r="B223" s="7"/>
       <c r="C223" s="8"/>
@@ -2788,7 +2786,7 @@
       <c r="G223" s="7"/>
       <c r="H223" s="8"/>
     </row>
-    <row r="224" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="224" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A224" s="7"/>
       <c r="B224" s="7"/>
       <c r="C224" s="8"/>
@@ -2798,7 +2796,7 @@
       <c r="G224" s="7"/>
       <c r="H224" s="8"/>
     </row>
-    <row r="225" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="225" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A225" s="7"/>
       <c r="B225" s="7"/>
       <c r="C225" s="8"/>
@@ -2808,7 +2806,7 @@
       <c r="G225" s="7"/>
       <c r="H225" s="8"/>
     </row>
-    <row r="226" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="226" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A226" s="7"/>
       <c r="B226" s="7"/>
       <c r="C226" s="8"/>
@@ -2818,7 +2816,7 @@
       <c r="G226" s="7"/>
       <c r="H226" s="8"/>
     </row>
-    <row r="227" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="227" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A227" s="7"/>
       <c r="B227" s="7"/>
       <c r="C227" s="8"/>
@@ -2828,7 +2826,7 @@
       <c r="G227" s="7"/>
       <c r="H227" s="8"/>
     </row>
-    <row r="228" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="228" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A228" s="7"/>
       <c r="B228" s="7"/>
       <c r="C228" s="8"/>
@@ -2838,7 +2836,7 @@
       <c r="G228" s="7"/>
       <c r="H228" s="8"/>
     </row>
-    <row r="229" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="229" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A229" s="7"/>
       <c r="B229" s="7"/>
       <c r="C229" s="8"/>
@@ -2848,7 +2846,7 @@
       <c r="G229" s="7"/>
       <c r="H229" s="8"/>
     </row>
-    <row r="230" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="230" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A230" s="7"/>
       <c r="B230" s="7"/>
       <c r="C230" s="8"/>
@@ -2858,7 +2856,7 @@
       <c r="G230" s="7"/>
       <c r="H230" s="8"/>
     </row>
-    <row r="231" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="231" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A231" s="7"/>
       <c r="B231" s="7"/>
       <c r="C231" s="8"/>
@@ -2868,7 +2866,7 @@
       <c r="G231" s="7"/>
       <c r="H231" s="8"/>
     </row>
-    <row r="232" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="232" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A232" s="7"/>
       <c r="B232" s="7"/>
       <c r="C232" s="8"/>
@@ -2878,7 +2876,7 @@
       <c r="G232" s="7"/>
       <c r="H232" s="8"/>
     </row>
-    <row r="233" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="233" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A233" s="7"/>
       <c r="B233" s="7"/>
       <c r="C233" s="8"/>
@@ -2888,7 +2886,7 @@
       <c r="G233" s="7"/>
       <c r="H233" s="8"/>
     </row>
-    <row r="234" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="234" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A234" s="7"/>
       <c r="B234" s="7"/>
       <c r="C234" s="8"/>
@@ -2898,7 +2896,7 @@
       <c r="G234" s="7"/>
       <c r="H234" s="8"/>
     </row>
-    <row r="235" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="235" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A235" s="7"/>
       <c r="B235" s="7"/>
       <c r="C235" s="8"/>
@@ -2908,7 +2906,7 @@
       <c r="G235" s="7"/>
       <c r="H235" s="8"/>
     </row>
-    <row r="236" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="236" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A236" s="7"/>
       <c r="B236" s="7"/>
       <c r="C236" s="8"/>
@@ -2918,7 +2916,7 @@
       <c r="G236" s="7"/>
       <c r="H236" s="8"/>
     </row>
-    <row r="237" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="237" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A237" s="7"/>
       <c r="B237" s="7"/>
       <c r="C237" s="8"/>
@@ -2928,7 +2926,7 @@
       <c r="G237" s="7"/>
       <c r="H237" s="8"/>
     </row>
-    <row r="238" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="238" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A238" s="7"/>
       <c r="B238" s="7"/>
       <c r="C238" s="8"/>
@@ -2938,7 +2936,7 @@
       <c r="G238" s="7"/>
       <c r="H238" s="8"/>
     </row>
-    <row r="239" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="239" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A239" s="7"/>
       <c r="B239" s="7"/>
       <c r="C239" s="8"/>
@@ -2948,7 +2946,7 @@
       <c r="G239" s="7"/>
       <c r="H239" s="8"/>
     </row>
-    <row r="240" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="240" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A240" s="7"/>
       <c r="B240" s="7"/>
       <c r="C240" s="8"/>
@@ -2958,7 +2956,7 @@
       <c r="G240" s="7"/>
       <c r="H240" s="8"/>
     </row>
-    <row r="241" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="241" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A241" s="7"/>
       <c r="B241" s="7"/>
       <c r="C241" s="8"/>
@@ -2968,7 +2966,7 @@
       <c r="G241" s="7"/>
       <c r="H241" s="8"/>
     </row>
-    <row r="242" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="242" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A242" s="7"/>
       <c r="B242" s="7"/>
       <c r="C242" s="8"/>
@@ -2978,7 +2976,7 @@
       <c r="G242" s="7"/>
       <c r="H242" s="8"/>
     </row>
-    <row r="243" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="243" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A243" s="7"/>
       <c r="B243" s="7"/>
       <c r="C243" s="8"/>
@@ -2988,7 +2986,7 @@
       <c r="G243" s="7"/>
       <c r="H243" s="8"/>
     </row>
-    <row r="244" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="244" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A244" s="7"/>
       <c r="B244" s="7"/>
       <c r="C244" s="8"/>
@@ -2998,7 +2996,7 @@
       <c r="G244" s="7"/>
       <c r="H244" s="8"/>
     </row>
-    <row r="245" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="245" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A245" s="7"/>
       <c r="B245" s="7"/>
       <c r="C245" s="8"/>
@@ -3008,7 +3006,7 @@
       <c r="G245" s="7"/>
       <c r="H245" s="8"/>
     </row>
-    <row r="246" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="246" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A246" s="7"/>
       <c r="B246" s="7"/>
       <c r="C246" s="8"/>
@@ -3018,7 +3016,7 @@
       <c r="G246" s="7"/>
       <c r="H246" s="8"/>
     </row>
-    <row r="247" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="247" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A247" s="7"/>
       <c r="B247" s="7"/>
       <c r="C247" s="8"/>
@@ -3028,7 +3026,7 @@
       <c r="G247" s="7"/>
       <c r="H247" s="8"/>
     </row>
-    <row r="248" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="248" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A248" s="7"/>
       <c r="B248" s="7"/>
       <c r="C248" s="8"/>
@@ -3038,7 +3036,7 @@
       <c r="G248" s="7"/>
       <c r="H248" s="8"/>
     </row>
-    <row r="249" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="249" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A249" s="7"/>
       <c r="B249" s="7"/>
       <c r="C249" s="8"/>
@@ -3048,7 +3046,7 @@
       <c r="G249" s="7"/>
       <c r="H249" s="8"/>
     </row>
-    <row r="250" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="250" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A250" s="7"/>
       <c r="B250" s="7"/>
       <c r="C250" s="8"/>
@@ -3058,7 +3056,7 @@
       <c r="G250" s="7"/>
       <c r="H250" s="8"/>
     </row>
-    <row r="251" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="251" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A251" s="7"/>
       <c r="B251" s="7"/>
       <c r="C251" s="8"/>
@@ -3068,7 +3066,7 @@
       <c r="G251" s="7"/>
       <c r="H251" s="8"/>
     </row>
-    <row r="252" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="252" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A252" s="7"/>
       <c r="B252" s="7"/>
       <c r="C252" s="8"/>
@@ -3078,7 +3076,7 @@
       <c r="G252" s="7"/>
       <c r="H252" s="8"/>
     </row>
-    <row r="253" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="253" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A253" s="7"/>
       <c r="B253" s="7"/>
       <c r="C253" s="8"/>
@@ -3088,7 +3086,7 @@
       <c r="G253" s="7"/>
       <c r="H253" s="8"/>
     </row>
-    <row r="254" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="254" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A254" s="7"/>
       <c r="B254" s="7"/>
       <c r="C254" s="8"/>
@@ -3098,7 +3096,7 @@
       <c r="G254" s="7"/>
       <c r="H254" s="8"/>
     </row>
-    <row r="255" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="255" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A255" s="7"/>
       <c r="B255" s="7"/>
       <c r="C255" s="8"/>
@@ -3108,7 +3106,7 @@
       <c r="G255" s="7"/>
       <c r="H255" s="8"/>
     </row>
-    <row r="256" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="256" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A256" s="7"/>
       <c r="B256" s="7"/>
       <c r="C256" s="8"/>
@@ -3118,7 +3116,7 @@
       <c r="G256" s="7"/>
       <c r="H256" s="8"/>
     </row>
-    <row r="257" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="257" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A257" s="7"/>
       <c r="B257" s="7"/>
       <c r="C257" s="8"/>
@@ -3128,7 +3126,7 @@
       <c r="G257" s="7"/>
       <c r="H257" s="8"/>
     </row>
-    <row r="258" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="258" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A258" s="7"/>
       <c r="B258" s="7"/>
       <c r="C258" s="8"/>
@@ -3138,7 +3136,7 @@
       <c r="G258" s="7"/>
       <c r="H258" s="8"/>
     </row>
-    <row r="259" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="259" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A259" s="7"/>
       <c r="B259" s="7"/>
       <c r="C259" s="8"/>
@@ -3148,7 +3146,7 @@
       <c r="G259" s="7"/>
       <c r="H259" s="8"/>
     </row>
-    <row r="260" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="260" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A260" s="7"/>
       <c r="B260" s="7"/>
       <c r="C260" s="8"/>
@@ -3158,7 +3156,7 @@
       <c r="G260" s="7"/>
       <c r="H260" s="8"/>
     </row>
-    <row r="261" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="261" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A261" s="7"/>
       <c r="B261" s="7"/>
       <c r="C261" s="8"/>
@@ -3168,7 +3166,7 @@
       <c r="G261" s="7"/>
       <c r="H261" s="8"/>
     </row>
-    <row r="262" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="262" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A262" s="7"/>
       <c r="B262" s="7"/>
       <c r="C262" s="8"/>
@@ -3178,7 +3176,7 @@
       <c r="G262" s="7"/>
       <c r="H262" s="8"/>
     </row>
-    <row r="263" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="263" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A263" s="7"/>
       <c r="B263" s="7"/>
       <c r="C263" s="8"/>
@@ -3188,7 +3186,7 @@
       <c r="G263" s="7"/>
       <c r="H263" s="8"/>
     </row>
-    <row r="264" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="264" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A264" s="7"/>
       <c r="B264" s="7"/>
       <c r="C264" s="8"/>
@@ -3198,7 +3196,7 @@
       <c r="G264" s="7"/>
       <c r="H264" s="8"/>
     </row>
-    <row r="265" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="265" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A265" s="7"/>
       <c r="B265" s="7"/>
       <c r="C265" s="8"/>
@@ -3208,7 +3206,7 @@
       <c r="G265" s="7"/>
       <c r="H265" s="8"/>
     </row>
-    <row r="266" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="266" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A266" s="7"/>
       <c r="B266" s="7"/>
       <c r="C266" s="8"/>
@@ -3218,7 +3216,7 @@
       <c r="G266" s="7"/>
       <c r="H266" s="8"/>
     </row>
-    <row r="267" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="267" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A267" s="7"/>
       <c r="B267" s="7"/>
       <c r="C267" s="8"/>
@@ -3228,7 +3226,7 @@
       <c r="G267" s="7"/>
       <c r="H267" s="8"/>
     </row>
-    <row r="268" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="268" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A268" s="7"/>
       <c r="B268" s="7"/>
       <c r="C268" s="8"/>
@@ -3238,7 +3236,7 @@
       <c r="G268" s="7"/>
       <c r="H268" s="8"/>
     </row>
-    <row r="269" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="269" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A269" s="7"/>
       <c r="B269" s="7"/>
       <c r="C269" s="8"/>
@@ -3248,7 +3246,7 @@
       <c r="G269" s="7"/>
       <c r="H269" s="8"/>
     </row>
-    <row r="270" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="270" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A270" s="7"/>
       <c r="B270" s="7"/>
       <c r="C270" s="8"/>
@@ -3258,7 +3256,7 @@
       <c r="G270" s="7"/>
       <c r="H270" s="8"/>
     </row>
-    <row r="271" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="271" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A271" s="7"/>
       <c r="B271" s="7"/>
       <c r="C271" s="8"/>
@@ -3268,7 +3266,7 @@
       <c r="G271" s="7"/>
       <c r="H271" s="8"/>
     </row>
-    <row r="272" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="272" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A272" s="7"/>
       <c r="B272" s="7"/>
       <c r="C272" s="8"/>
@@ -3278,7 +3276,7 @@
       <c r="G272" s="7"/>
       <c r="H272" s="8"/>
     </row>
-    <row r="273" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="273" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A273" s="7"/>
       <c r="B273" s="7"/>
       <c r="C273" s="8"/>
@@ -3288,7 +3286,7 @@
       <c r="G273" s="7"/>
       <c r="H273" s="8"/>
     </row>
-    <row r="274" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="274" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A274" s="7"/>
       <c r="B274" s="7"/>
       <c r="C274" s="8"/>
@@ -3298,7 +3296,7 @@
       <c r="G274" s="7"/>
       <c r="H274" s="8"/>
     </row>
-    <row r="275" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="275" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A275" s="7"/>
       <c r="B275" s="7"/>
       <c r="C275" s="8"/>
@@ -3308,7 +3306,7 @@
       <c r="G275" s="7"/>
       <c r="H275" s="8"/>
     </row>
-    <row r="276" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="276" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A276" s="7"/>
       <c r="B276" s="7"/>
       <c r="C276" s="8"/>
@@ -3318,7 +3316,7 @@
       <c r="G276" s="7"/>
       <c r="H276" s="8"/>
     </row>
-    <row r="277" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="277" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A277" s="7"/>
       <c r="B277" s="7"/>
       <c r="C277" s="8"/>
@@ -3328,7 +3326,7 @@
       <c r="G277" s="7"/>
       <c r="H277" s="8"/>
     </row>
-    <row r="278" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="278" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A278" s="7"/>
       <c r="B278" s="7"/>
       <c r="C278" s="8"/>
@@ -3338,7 +3336,7 @@
       <c r="G278" s="7"/>
       <c r="H278" s="8"/>
     </row>
-    <row r="279" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="279" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A279" s="7"/>
       <c r="B279" s="7"/>
       <c r="C279" s="8"/>
@@ -3348,7 +3346,7 @@
       <c r="G279" s="7"/>
       <c r="H279" s="8"/>
     </row>
-    <row r="280" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="280" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A280" s="7"/>
       <c r="B280" s="7"/>
       <c r="C280" s="8"/>
@@ -3358,7 +3356,7 @@
       <c r="G280" s="7"/>
       <c r="H280" s="8"/>
     </row>
-    <row r="281" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="281" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A281" s="7"/>
       <c r="B281" s="7"/>
       <c r="C281" s="8"/>
@@ -3368,7 +3366,7 @@
       <c r="G281" s="7"/>
       <c r="H281" s="8"/>
     </row>
-    <row r="282" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="282" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A282" s="7"/>
       <c r="B282" s="7"/>
       <c r="C282" s="8"/>
@@ -3378,7 +3376,7 @@
       <c r="G282" s="7"/>
       <c r="H282" s="8"/>
     </row>
-    <row r="283" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="283" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A283" s="7"/>
       <c r="B283" s="7"/>
       <c r="C283" s="8"/>
@@ -3388,7 +3386,7 @@
       <c r="G283" s="7"/>
       <c r="H283" s="8"/>
     </row>
-    <row r="284" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="284" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A284" s="7"/>
       <c r="B284" s="7"/>
       <c r="C284" s="8"/>
@@ -3398,7 +3396,7 @@
       <c r="G284" s="7"/>
       <c r="H284" s="8"/>
     </row>
-    <row r="285" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="285" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A285" s="7"/>
       <c r="B285" s="7"/>
       <c r="C285" s="8"/>
@@ -3408,7 +3406,7 @@
       <c r="G285" s="7"/>
       <c r="H285" s="8"/>
     </row>
-    <row r="286" spans="1:8" s="1" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="286" customHeight="1" ht="40.9" customFormat="1" s="1">
       <c r="A286" s="7"/>
       <c r="B286" s="7"/>
       <c r="C286" s="8"/>

</xml_diff>